<commit_message>
added missing column header in test pack
</commit_message>
<xml_diff>
--- a/tool/e2e-tests/test-packs/Test Pack - Script Types - Not Allowed.xlsx
+++ b/tool/e2e-tests/test-packs/Test Pack - Script Types - Not Allowed.xlsx
@@ -9,7 +9,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathew.arnold\electronic-prescription-service-api\tool\e2e-tests\test-packs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF2F34A-DE01-4195-96D7-8D04803DCCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2469513C-2FB1-4F6A-B3CF-07ED4F2397E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="16186" firstSheet="1" activeTab="1" xr2:uid="{DE2866F1-D839-4AD2-B338-FF4A1D84F7C7}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="165">
   <si>
     <t>Only one organisation is supported</t>
   </si>
@@ -531,6 +531,9 @@
   </si>
   <si>
     <t>P1</t>
+  </si>
+  <si>
+    <t>Nominated Pharmacy Type</t>
   </si>
 </sst>
 </file>
@@ -1009,8 +1012,8 @@
   <dimension ref="A1:V81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E62"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
@@ -1052,7 +1055,9 @@
       <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
@@ -4438,26 +4443,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="76e91428-a7f3-4551-8ad9-355bcde117c2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5b69da58-499a-4190-98d9-528841fe850b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010077F18FD3DE1A9F46B48F2CEB8D58E8DE" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29bbfc33a20b984a6bd9df737087a05c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5b69da58-499a-4190-98d9-528841fe850b" xmlns:ns3="76e91428-a7f3-4551-8ad9-355bcde117c2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d695bf3dcfa2ca9c872e2cc9249639" ns2:_="" ns3:_="">
     <xsd:import namespace="5b69da58-499a-4190-98d9-528841fe850b"/>
@@ -4668,26 +4653,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EAD036D-F34A-4E5B-9E8E-5D20D0D65AE2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="76e91428-a7f3-4551-8ad9-355bcde117c2"/>
-    <ds:schemaRef ds:uri="5b69da58-499a-4190-98d9-528841fe850b"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1992767-8B66-4024-9F8C-CD8162B305A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="76e91428-a7f3-4551-8ad9-355bcde117c2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5b69da58-499a-4190-98d9-528841fe850b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51687A1D-BCE9-4F18-8CFB-7F030D88E905}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4704,4 +4690,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1992767-8B66-4024-9F8C-CD8162B305A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7EAD036D-F34A-4E5B-9E8E-5D20D0D65AE2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="76e91428-a7f3-4551-8ad9-355bcde117c2"/>
+    <ds:schemaRef ds:uri="5b69da58-499a-4190-98d9-528841fe850b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>